<commit_message>
fixing key format errors in 2002
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_2002.xlsx
+++ b/bioSample/bioSample_2002.xlsx
@@ -127,7 +127,7 @@
     <t xml:space="preserve">CNAG_02364</t>
   </si>
   <si>
-    <t xml:space="preserve">1.24.17</t>
+    <t xml:space="preserve">01.24.17</t>
   </si>
   <si>
     <t xml:space="preserve">TDY2017</t>
@@ -178,6 +178,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -261,8 +262,8 @@
   </sheetPr>
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -274,7 +275,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="9.07"/>

</xml_diff>

<commit_message>
fixed s1cndasamplenumber in s1CDNASample_J.PLAGGENBERG_05.30.19.xlsx and update marker info in 2002
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_2002.xlsx
+++ b/bioSample/bioSample_2002.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="48">
   <si>
     <t xml:space="preserve">harvestDate</t>
   </si>
@@ -94,13 +94,13 @@
     <t xml:space="preserve">G418</t>
   </si>
   <si>
+    <t xml:space="preserve">NAT</t>
+  </si>
+  <si>
     <t xml:space="preserve">TDY1700</t>
   </si>
   <si>
     <t xml:space="preserve">CNAG_00156</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAT</t>
   </si>
   <si>
     <t xml:space="preserve">TDY1936</t>
@@ -262,8 +262,8 @@
   </sheetPr>
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N6" activeCellId="0" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -480,6 +480,9 @@
       <c r="M5" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="N5" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -521,6 +524,9 @@
       <c r="M6" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="N6" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -562,6 +568,9 @@
       <c r="M7" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="N7" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -580,10 +589,10 @@
         <v>17</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>17</v>
@@ -601,7 +610,7 @@
         <v>1</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -621,10 +630,10 @@
         <v>17</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>17</v>
@@ -642,7 +651,7 @@
         <v>2</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -662,10 +671,10 @@
         <v>17</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>17</v>
@@ -683,7 +692,7 @@
         <v>3</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -970,7 +979,7 @@
         <v>1</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1011,7 +1020,7 @@
         <v>2</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1052,7 +1061,7 @@
         <v>3</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1093,7 +1102,7 @@
         <v>1</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1134,7 +1143,7 @@
         <v>2</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1175,7 +1184,7 @@
         <v>3</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1330,7 +1339,7 @@
         <v>1</v>
       </c>
       <c r="M26" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N26" s="0" t="s">
         <v>23</v>
@@ -1374,7 +1383,7 @@
         <v>2</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N27" s="0" t="s">
         <v>23</v>
@@ -1418,7 +1427,7 @@
         <v>3</v>
       </c>
       <c r="M28" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N28" s="0" t="s">
         <v>23</v>
@@ -1465,7 +1474,7 @@
         <v>23</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1509,7 +1518,7 @@
         <v>23</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1553,7 +1562,7 @@
         <v>23</v>
       </c>
       <c r="N31" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1717,7 +1726,7 @@
         <v>1</v>
       </c>
       <c r="M35" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1758,7 +1767,7 @@
         <v>2</v>
       </c>
       <c r="M36" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1799,7 +1808,7 @@
         <v>3</v>
       </c>
       <c r="M37" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1840,7 +1849,7 @@
         <v>1</v>
       </c>
       <c r="M38" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1881,7 +1890,7 @@
         <v>2</v>
       </c>
       <c r="M39" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1922,7 +1931,7 @@
         <v>3</v>
       </c>
       <c r="M40" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1963,7 +1972,7 @@
         <v>1</v>
       </c>
       <c r="M41" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2004,7 +2013,7 @@
         <v>2</v>
       </c>
       <c r="M42" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2045,7 +2054,7 @@
         <v>3</v>
       </c>
       <c r="M43" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2212,7 +2221,7 @@
         <v>23</v>
       </c>
       <c r="N47" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2256,7 +2265,7 @@
         <v>23</v>
       </c>
       <c r="N48" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2300,7 +2309,7 @@
         <v>23</v>
       </c>
       <c r="N49" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>